<commit_message>
updated flow and visual (in progress)
added azure storage to flow. added output from flow to twb but not created visuals yets
</commit_message>
<xml_diff>
--- a/data/Azure regions mapped to city.xlsx
+++ b/data/Azure regions mapped to city.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/183a3132ccad9910/Documents/GitHub/Cloud-Comparison/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="8_{E3D34594-E486-4D61-85BD-D8B880735B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9E74736-C5BA-4AEC-90C6-0018A37C7303}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{E3D34594-E486-4D61-85BD-D8B880735B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A45E1FFD-E569-47BD-A071-3C03C9C4F3A2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{5B3FF079-FECF-4832-A87F-15B323B68748}"/>
   </bookViews>
@@ -312,12 +312,6 @@
     <t>JA East</t>
   </si>
   <si>
-    <t>KP Central</t>
-  </si>
-  <si>
-    <t>KP South</t>
-  </si>
-  <si>
     <t>SE Central</t>
   </si>
   <si>
@@ -370,6 +364,12 @@
   </si>
   <si>
     <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>KR Central</t>
+  </si>
+  <si>
+    <t>KR South</t>
   </si>
 </sst>
 </file>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E4CED4-90A3-4F30-B342-E26C7FC6A50E}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,7 +792,7 @@
         <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>73</v>
@@ -805,7 +805,7 @@
         <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>74</v>
@@ -899,7 +899,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -912,7 +912,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
         <v>52</v>
@@ -977,7 +977,7 @@
         <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>67</v>
@@ -990,7 +990,7 @@
         <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>68</v>
@@ -1023,7 +1023,7 @@
         <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>65</v>
@@ -1036,7 +1036,7 @@
         <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>66</v>
@@ -1046,10 +1046,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>55</v>
@@ -1062,7 +1062,7 @@
         <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>58</v>
@@ -1072,10 +1072,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>63</v>
@@ -1088,7 +1088,7 @@
         <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>64</v>
@@ -1101,7 +1101,7 @@
         <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>59</v>
@@ -1114,10 +1114,10 @@
         <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1125,7 +1125,7 @@
         <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>57</v>
@@ -1133,10 +1133,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>60</v>
@@ -1144,10 +1144,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>61</v>
@@ -1161,7 +1161,7 @@
         <v>50</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -1175,10 +1175,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>70</v>
@@ -1186,10 +1186,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>71</v>
@@ -1328,10 +1328,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>53</v>
@@ -1339,10 +1339,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>54</v>

</xml_diff>